<commit_message>
Added NaN expection and sample data
</commit_message>
<xml_diff>
--- a/input_sheet.xlsx
+++ b/input_sheet.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/partharora/Desktop/bot-test/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/partharora/github/GT-RA-Log-Bot/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBAF6AC1-9471-B746-8509-2EDCCC30A687}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{043B82E5-C7D4-A242-AAA1-946C5E084878}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="16680" xr2:uid="{F053D245-90CA-5A47-B0CD-784ADE272EB4}"/>
+    <workbookView xWindow="0" yWindow="720" windowWidth="29400" windowHeight="18400" xr2:uid="{F053D245-90CA-5A47-B0CD-784ADE272EB4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="91">
   <si>
     <t>Interaction Log</t>
   </si>
@@ -138,13 +138,184 @@
   </si>
   <si>
     <t>John Doe</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>Ivan Wang</t>
+  </si>
+  <si>
+    <t>Matthew Lei</t>
+  </si>
+  <si>
+    <t>Alex Yang</t>
+  </si>
+  <si>
+    <t>Rohan Ravula</t>
+  </si>
+  <si>
+    <t>Karthik Kundurthy</t>
+  </si>
+  <si>
+    <t>Nihit Agarwal</t>
+  </si>
+  <si>
+    <t>Shriyanshu Kode</t>
+  </si>
+  <si>
+    <t>Jatong Su</t>
+  </si>
+  <si>
+    <t>Jeremy Wang</t>
+  </si>
+  <si>
+    <t>Edward Chen</t>
+  </si>
+  <si>
+    <t>Shiv Patel</t>
+  </si>
+  <si>
+    <t>Anthony Hoyt</t>
+  </si>
+  <si>
+    <t>Michael Camacho</t>
+  </si>
+  <si>
+    <t>Davis Lomenick</t>
+  </si>
+  <si>
+    <t>Liam Smith</t>
+  </si>
+  <si>
+    <t>James Keller</t>
+  </si>
+  <si>
+    <t>Jackson Hogan</t>
+  </si>
+  <si>
+    <t>Cynthia Li</t>
+  </si>
+  <si>
+    <t>Sophia Garcia</t>
+  </si>
+  <si>
+    <t>Chandler Fortune</t>
+  </si>
+  <si>
+    <t>Wendy Sun</t>
+  </si>
+  <si>
+    <t>Brian Goldblatt</t>
+  </si>
+  <si>
+    <t>William Dannelly</t>
+  </si>
+  <si>
+    <t>Vincent Panunzio</t>
+  </si>
+  <si>
+    <t>Liam Watson</t>
+  </si>
+  <si>
+    <t>Suvrat Jain</t>
+  </si>
+  <si>
+    <t>Aditya Palliyil</t>
+  </si>
+  <si>
+    <t>Avinash Palliyil</t>
+  </si>
+  <si>
+    <t>Cem Kocer</t>
+  </si>
+  <si>
+    <t>Adhira Choudhury</t>
+  </si>
+  <si>
+    <t>Unnathi Kumar</t>
+  </si>
+  <si>
+    <t>Khushi Gupta</t>
+  </si>
+  <si>
+    <t>Muskaan Muskaan</t>
+  </si>
+  <si>
+    <t>Hoang-An Pham</t>
+  </si>
+  <si>
+    <t>Joshua Reese</t>
+  </si>
+  <si>
+    <t>Griffin Wagner</t>
+  </si>
+  <si>
+    <t>Evan Sanchez</t>
+  </si>
+  <si>
+    <t>Aishat Adeboye</t>
+  </si>
+  <si>
+    <t>Alyssa Lawji</t>
+  </si>
+  <si>
+    <t>Zeynab Sow</t>
+  </si>
+  <si>
+    <t>Rushda Umrani</t>
+  </si>
+  <si>
+    <t>Jordan Beiler</t>
+  </si>
+  <si>
+    <t>Vignesh Sekar</t>
+  </si>
+  <si>
+    <t>Jack Hayley</t>
+  </si>
+  <si>
+    <t>Gate Tangchartsiri</t>
+  </si>
+  <si>
+    <t>Mahta Tavafoghi</t>
+  </si>
+  <si>
+    <t>Nashad Mohamed</t>
+  </si>
+  <si>
+    <t>Elayna Pak</t>
+  </si>
+  <si>
+    <t>Catherine McCoy</t>
+  </si>
+  <si>
+    <t>Isabelle Jungwirth</t>
+  </si>
+  <si>
+    <t>Tesfanesh Keith</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>E</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>-</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -171,6 +342,13 @@
     <font>
       <sz val="18"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -304,7 +482,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -333,14 +511,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -352,6 +522,19 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -668,10 +851,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ADE7FBAC-F328-B14F-AF70-DCD7577D430D}">
-  <dimension ref="A1:M32"/>
+  <dimension ref="A1:M57"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="113" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -691,28 +874,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="43" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="16"/>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
-      <c r="E1" s="16"/>
-      <c r="F1" s="16"/>
-      <c r="G1" s="16"/>
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="12"/>
+      <c r="F1" s="12"/>
+      <c r="G1" s="12"/>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="B2" s="14" t="s">
+      <c r="B2" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="C2" s="14"/>
-      <c r="D2" s="14" t="s">
+      <c r="C2" s="17"/>
+      <c r="D2" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="E2" s="14"/>
+      <c r="E2" s="17"/>
       <c r="F2" s="7" t="s">
         <v>26</v>
       </c>
@@ -722,14 +905,14 @@
       <c r="A3" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="B3" s="15" t="s">
+      <c r="B3" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="C3" s="15"/>
-      <c r="D3" s="13" t="s">
+      <c r="C3" s="18"/>
+      <c r="D3" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="E3" s="13"/>
+      <c r="E3" s="16"/>
       <c r="F3" s="11">
         <v>6</v>
       </c>
@@ -757,20 +940,20 @@
       <c r="G4" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="J4" s="17" t="s">
+      <c r="J4" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="K4" s="18"/>
-      <c r="L4" s="18" t="s">
+      <c r="K4" s="14"/>
+      <c r="L4" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="M4" s="19"/>
+      <c r="M4" s="15"/>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>33</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="1">
         <v>602</v>
       </c>
       <c r="C5" t="s">
@@ -805,13 +988,21 @@
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A6" s="10"/>
-      <c r="B6" s="10"/>
-      <c r="C6" s="10"/>
-      <c r="D6" s="12"/>
-      <c r="E6" s="10"/>
+      <c r="A6" s="19" t="s">
+        <v>35</v>
+      </c>
+      <c r="B6" s="19">
+        <v>602</v>
+      </c>
+      <c r="C6" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6" s="20"/>
+      <c r="E6" s="9"/>
       <c r="F6" s="10"/>
-      <c r="G6" s="10"/>
+      <c r="G6" s="10" t="s">
+        <v>90</v>
+      </c>
       <c r="H6" s="1" t="s">
         <v>32</v>
       </c>
@@ -829,13 +1020,21 @@
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A7" s="10"/>
-      <c r="B7" s="10"/>
-      <c r="C7" s="10"/>
-      <c r="D7" s="12"/>
-      <c r="E7" s="10"/>
+      <c r="A7" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="B7" s="19">
+        <v>602</v>
+      </c>
+      <c r="C7" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="D7" s="20"/>
+      <c r="E7" s="9"/>
       <c r="F7" s="10"/>
-      <c r="G7" s="10"/>
+      <c r="G7" s="10" t="s">
+        <v>90</v>
+      </c>
       <c r="J7" s="2" t="s">
         <v>12</v>
       </c>
@@ -850,13 +1049,21 @@
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A8" s="9"/>
-      <c r="B8" s="9"/>
-      <c r="C8" s="9"/>
-      <c r="D8" s="9"/>
+      <c r="A8" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="B8" s="19">
+        <v>602</v>
+      </c>
+      <c r="C8" s="19" t="s">
+        <v>86</v>
+      </c>
+      <c r="D8" s="20"/>
       <c r="E8" s="9"/>
-      <c r="F8" s="9"/>
-      <c r="G8" s="9"/>
+      <c r="F8" s="10"/>
+      <c r="G8" s="10" t="s">
+        <v>90</v>
+      </c>
       <c r="J8" s="2" t="s">
         <v>10</v>
       </c>
@@ -871,13 +1078,21 @@
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A9" s="9"/>
-      <c r="B9" s="9"/>
-      <c r="C9" s="9"/>
+      <c r="A9" s="19" t="s">
+        <v>27</v>
+      </c>
+      <c r="B9" s="19">
+        <v>602</v>
+      </c>
+      <c r="C9" s="19" t="s">
+        <v>87</v>
+      </c>
       <c r="D9" s="9"/>
       <c r="E9" s="9"/>
       <c r="F9" s="9"/>
-      <c r="G9" s="9"/>
+      <c r="G9" s="10" t="s">
+        <v>90</v>
+      </c>
       <c r="J9" s="2" t="s">
         <v>14</v>
       </c>
@@ -892,13 +1107,21 @@
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A10" s="9"/>
-      <c r="B10" s="9"/>
-      <c r="C10" s="9"/>
+      <c r="A10" s="19" t="s">
+        <v>38</v>
+      </c>
+      <c r="B10" s="19">
+        <v>604</v>
+      </c>
+      <c r="C10" s="19" t="s">
+        <v>8</v>
+      </c>
       <c r="D10" s="9"/>
       <c r="E10" s="9"/>
       <c r="F10" s="9"/>
-      <c r="G10" s="9"/>
+      <c r="G10" s="10" t="s">
+        <v>90</v>
+      </c>
       <c r="J10" s="4" t="s">
         <v>13</v>
       </c>
@@ -913,212 +1136,825 @@
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A11" s="9"/>
-      <c r="B11" s="9"/>
-      <c r="C11" s="9"/>
+      <c r="A11" s="19" t="s">
+        <v>39</v>
+      </c>
+      <c r="B11" s="19">
+        <v>604</v>
+      </c>
+      <c r="C11" s="19" t="s">
+        <v>34</v>
+      </c>
       <c r="D11" s="9"/>
       <c r="E11" s="9"/>
       <c r="F11" s="9"/>
-      <c r="G11" s="9"/>
+      <c r="G11" s="10" t="s">
+        <v>90</v>
+      </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A12" s="9"/>
-      <c r="B12" s="9"/>
-      <c r="C12" s="9"/>
-      <c r="D12" s="9"/>
+      <c r="A12" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="B12" s="19">
+        <v>604</v>
+      </c>
+      <c r="C12" s="19" t="s">
+        <v>86</v>
+      </c>
+      <c r="D12" s="20"/>
       <c r="E12" s="9"/>
       <c r="F12" s="9"/>
-      <c r="G12" s="9"/>
+      <c r="G12" s="10" t="s">
+        <v>90</v>
+      </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A13" s="9"/>
-      <c r="B13" s="9"/>
-      <c r="C13" s="9"/>
+      <c r="A13" s="19" t="s">
+        <v>41</v>
+      </c>
+      <c r="B13" s="19">
+        <v>604</v>
+      </c>
+      <c r="C13" s="19" t="s">
+        <v>87</v>
+      </c>
       <c r="D13" s="9"/>
       <c r="E13" s="9"/>
       <c r="F13" s="9"/>
-      <c r="G13" s="9"/>
+      <c r="G13" s="10" t="s">
+        <v>90</v>
+      </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A14" s="9"/>
-      <c r="B14" s="9"/>
-      <c r="C14" s="9"/>
+      <c r="A14" s="19" t="s">
+        <v>42</v>
+      </c>
+      <c r="B14" s="19">
+        <v>605</v>
+      </c>
+      <c r="C14" s="19" t="s">
+        <v>8</v>
+      </c>
       <c r="D14" s="9"/>
       <c r="E14" s="9"/>
       <c r="F14" s="9"/>
-      <c r="G14" s="9"/>
+      <c r="G14" s="10" t="s">
+        <v>90</v>
+      </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A15" s="9"/>
-      <c r="B15" s="9"/>
-      <c r="C15" s="9"/>
+      <c r="A15" s="19" t="s">
+        <v>43</v>
+      </c>
+      <c r="B15" s="19">
+        <v>605</v>
+      </c>
+      <c r="C15" s="19" t="s">
+        <v>34</v>
+      </c>
       <c r="D15" s="9"/>
       <c r="E15" s="9"/>
       <c r="F15" s="9"/>
-      <c r="G15" s="9"/>
+      <c r="G15" s="10" t="s">
+        <v>90</v>
+      </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A16" s="9"/>
-      <c r="B16" s="9"/>
-      <c r="C16" s="9"/>
+      <c r="A16" s="19" t="s">
+        <v>44</v>
+      </c>
+      <c r="B16" s="19">
+        <v>605</v>
+      </c>
+      <c r="C16" s="19" t="s">
+        <v>86</v>
+      </c>
       <c r="D16" s="9"/>
       <c r="E16" s="9"/>
       <c r="F16" s="9"/>
-      <c r="G16" s="9"/>
+      <c r="G16" s="10" t="s">
+        <v>90</v>
+      </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A17" s="9"/>
-      <c r="B17" s="9"/>
-      <c r="C17" s="9"/>
+      <c r="A17" s="19" t="s">
+        <v>45</v>
+      </c>
+      <c r="B17" s="19">
+        <v>605</v>
+      </c>
+      <c r="C17" s="19" t="s">
+        <v>87</v>
+      </c>
       <c r="D17" s="9"/>
       <c r="E17" s="9"/>
       <c r="F17" s="9"/>
-      <c r="G17" s="9"/>
+      <c r="G17" s="10" t="s">
+        <v>90</v>
+      </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A18" s="9"/>
-      <c r="B18" s="9"/>
-      <c r="C18" s="9"/>
+      <c r="A18" s="19" t="s">
+        <v>46</v>
+      </c>
+      <c r="B18" s="19">
+        <v>606</v>
+      </c>
+      <c r="C18" s="19" t="s">
+        <v>8</v>
+      </c>
       <c r="D18" s="9"/>
       <c r="E18" s="9"/>
       <c r="F18" s="9"/>
-      <c r="G18" s="9"/>
+      <c r="G18" s="10" t="s">
+        <v>90</v>
+      </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A19" s="9"/>
-      <c r="B19" s="9"/>
-      <c r="C19" s="9"/>
-      <c r="D19" s="9"/>
-      <c r="E19" s="9"/>
-      <c r="F19" s="9"/>
-      <c r="G19" s="9"/>
+      <c r="A19" s="19" t="s">
+        <v>47</v>
+      </c>
+      <c r="B19" s="19">
+        <v>606</v>
+      </c>
+      <c r="C19" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="D19" s="20">
+        <v>45181</v>
+      </c>
+      <c r="E19" s="9">
+        <v>1</v>
+      </c>
+      <c r="F19" s="9">
+        <v>4</v>
+      </c>
+      <c r="G19" s="10" t="s">
+        <v>90</v>
+      </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A20" s="9"/>
-      <c r="B20" s="9"/>
-      <c r="C20" s="9"/>
+      <c r="A20" s="19" t="s">
+        <v>48</v>
+      </c>
+      <c r="B20" s="19">
+        <v>606</v>
+      </c>
+      <c r="C20" s="19" t="s">
+        <v>86</v>
+      </c>
       <c r="D20" s="9"/>
       <c r="E20" s="9"/>
       <c r="F20" s="9"/>
-      <c r="G20" s="9"/>
+      <c r="G20" s="10" t="s">
+        <v>90</v>
+      </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A21" s="9"/>
-      <c r="B21" s="9"/>
-      <c r="C21" s="9"/>
+      <c r="A21" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="B21" s="19">
+        <v>606</v>
+      </c>
+      <c r="C21" s="19" t="s">
+        <v>87</v>
+      </c>
       <c r="D21" s="9"/>
       <c r="E21" s="9"/>
       <c r="F21" s="9"/>
-      <c r="G21" s="9"/>
+      <c r="G21" s="10" t="s">
+        <v>90</v>
+      </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A22" s="9"/>
-      <c r="B22" s="9"/>
-      <c r="C22" s="9"/>
+      <c r="A22" s="19" t="s">
+        <v>50</v>
+      </c>
+      <c r="B22" s="19">
+        <v>606</v>
+      </c>
+      <c r="C22" s="19" t="s">
+        <v>88</v>
+      </c>
       <c r="D22" s="9"/>
       <c r="E22" s="9"/>
       <c r="F22" s="9"/>
-      <c r="G22" s="9"/>
+      <c r="G22" s="10" t="s">
+        <v>90</v>
+      </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A23" s="9"/>
-      <c r="B23" s="9"/>
-      <c r="C23" s="9"/>
+      <c r="A23" s="19" t="s">
+        <v>51</v>
+      </c>
+      <c r="B23" s="19">
+        <v>606</v>
+      </c>
+      <c r="C23" s="19" t="s">
+        <v>89</v>
+      </c>
       <c r="D23" s="9"/>
       <c r="E23" s="9"/>
       <c r="F23" s="9"/>
-      <c r="G23" s="9"/>
+      <c r="G23" s="10" t="s">
+        <v>90</v>
+      </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A24" s="9"/>
-      <c r="B24" s="9"/>
-      <c r="C24" s="9"/>
+      <c r="A24" s="19" t="s">
+        <v>52</v>
+      </c>
+      <c r="B24" s="19">
+        <v>608</v>
+      </c>
+      <c r="C24" s="19" t="s">
+        <v>8</v>
+      </c>
       <c r="D24" s="9"/>
       <c r="E24" s="9"/>
       <c r="F24" s="9"/>
-      <c r="G24" s="9"/>
+      <c r="G24" s="10" t="s">
+        <v>90</v>
+      </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A25" s="9"/>
-      <c r="B25" s="9"/>
-      <c r="C25" s="9"/>
+      <c r="A25" s="19" t="s">
+        <v>53</v>
+      </c>
+      <c r="B25" s="19">
+        <v>608</v>
+      </c>
+      <c r="C25" s="19" t="s">
+        <v>34</v>
+      </c>
       <c r="D25" s="9"/>
       <c r="E25" s="9"/>
       <c r="F25" s="9"/>
-      <c r="G25" s="9"/>
+      <c r="G25" s="10" t="s">
+        <v>90</v>
+      </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A26" s="9"/>
-      <c r="B26" s="9"/>
-      <c r="C26" s="9"/>
-      <c r="D26" s="9"/>
-      <c r="E26" s="9"/>
-      <c r="F26" s="9"/>
-      <c r="G26" s="9"/>
+      <c r="A26" s="19" t="s">
+        <v>54</v>
+      </c>
+      <c r="B26" s="19">
+        <v>608</v>
+      </c>
+      <c r="C26" s="19" t="s">
+        <v>86</v>
+      </c>
+      <c r="D26" s="20">
+        <v>45181</v>
+      </c>
+      <c r="E26" s="9">
+        <v>1</v>
+      </c>
+      <c r="F26" s="9">
+        <v>3</v>
+      </c>
+      <c r="G26" s="10" t="s">
+        <v>90</v>
+      </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A27" s="9"/>
-      <c r="B27" s="9"/>
-      <c r="C27" s="9"/>
+      <c r="A27" s="19" t="s">
+        <v>55</v>
+      </c>
+      <c r="B27" s="19">
+        <v>608</v>
+      </c>
+      <c r="C27" s="19" t="s">
+        <v>87</v>
+      </c>
       <c r="D27" s="9"/>
       <c r="E27" s="9"/>
       <c r="F27" s="9"/>
-      <c r="G27" s="9"/>
+      <c r="G27" s="10" t="s">
+        <v>90</v>
+      </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A28" s="9"/>
-      <c r="B28" s="9"/>
-      <c r="C28" s="9"/>
+      <c r="A28" s="19" t="s">
+        <v>56</v>
+      </c>
+      <c r="B28" s="19">
+        <v>612</v>
+      </c>
+      <c r="C28" s="19" t="s">
+        <v>8</v>
+      </c>
       <c r="D28" s="9"/>
       <c r="E28" s="9"/>
       <c r="F28" s="9"/>
-      <c r="G28" s="9"/>
+      <c r="G28" s="10" t="s">
+        <v>90</v>
+      </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A29" s="9"/>
-      <c r="B29" s="9"/>
-      <c r="C29" s="9"/>
+      <c r="A29" s="19" t="s">
+        <v>57</v>
+      </c>
+      <c r="B29" s="19">
+        <v>612</v>
+      </c>
+      <c r="C29" s="19" t="s">
+        <v>34</v>
+      </c>
       <c r="D29" s="9"/>
       <c r="E29" s="9"/>
       <c r="F29" s="9"/>
-      <c r="G29" s="9"/>
+      <c r="G29" s="10" t="s">
+        <v>90</v>
+      </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A30" s="9"/>
-      <c r="B30" s="9"/>
-      <c r="C30" s="9"/>
+      <c r="A30" s="19" t="s">
+        <v>58</v>
+      </c>
+      <c r="B30" s="19">
+        <v>612</v>
+      </c>
+      <c r="C30" s="19" t="s">
+        <v>86</v>
+      </c>
       <c r="D30" s="9"/>
       <c r="E30" s="9"/>
       <c r="F30" s="9"/>
-      <c r="G30" s="9"/>
+      <c r="G30" s="10" t="s">
+        <v>90</v>
+      </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A31" s="9"/>
-      <c r="B31" s="9"/>
-      <c r="C31" s="9"/>
+      <c r="A31" s="19" t="s">
+        <v>59</v>
+      </c>
+      <c r="B31" s="19">
+        <v>612</v>
+      </c>
+      <c r="C31" s="19" t="s">
+        <v>87</v>
+      </c>
       <c r="D31" s="9"/>
       <c r="E31" s="9"/>
       <c r="F31" s="9"/>
-      <c r="G31" s="9"/>
+      <c r="G31" s="10" t="s">
+        <v>90</v>
+      </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A32" s="9"/>
-      <c r="B32" s="9"/>
-      <c r="C32" s="9"/>
+      <c r="A32" s="19" t="s">
+        <v>60</v>
+      </c>
+      <c r="B32" s="19">
+        <v>613</v>
+      </c>
+      <c r="C32" s="19" t="s">
+        <v>8</v>
+      </c>
       <c r="D32" s="9"/>
       <c r="E32" s="9"/>
       <c r="F32" s="9"/>
-      <c r="G32" s="9"/>
+      <c r="G32" s="10" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A33" s="19" t="s">
+        <v>61</v>
+      </c>
+      <c r="B33" s="19">
+        <v>613</v>
+      </c>
+      <c r="C33" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="D33" s="9"/>
+      <c r="E33" s="9"/>
+      <c r="F33" s="9"/>
+      <c r="G33" s="10" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A34" s="19" t="s">
+        <v>62</v>
+      </c>
+      <c r="B34" s="19">
+        <v>613</v>
+      </c>
+      <c r="C34" s="19" t="s">
+        <v>86</v>
+      </c>
+      <c r="D34" s="9"/>
+      <c r="E34" s="9"/>
+      <c r="F34" s="9"/>
+      <c r="G34" s="10" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A35" s="19" t="s">
+        <v>63</v>
+      </c>
+      <c r="B35" s="19">
+        <v>613</v>
+      </c>
+      <c r="C35" s="19" t="s">
+        <v>87</v>
+      </c>
+      <c r="D35" s="9"/>
+      <c r="E35" s="9"/>
+      <c r="F35" s="9"/>
+      <c r="G35" s="10" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A36" s="19" t="s">
+        <v>64</v>
+      </c>
+      <c r="B36" s="19">
+        <v>614</v>
+      </c>
+      <c r="C36" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="D36" s="9"/>
+      <c r="E36" s="9"/>
+      <c r="F36" s="9"/>
+      <c r="G36" s="10" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A37" s="19" t="s">
+        <v>65</v>
+      </c>
+      <c r="B37" s="19">
+        <v>614</v>
+      </c>
+      <c r="C37" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="D37" s="9"/>
+      <c r="E37" s="9"/>
+      <c r="F37" s="9"/>
+      <c r="G37" s="10" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A38" s="19" t="s">
+        <v>66</v>
+      </c>
+      <c r="B38" s="19">
+        <v>614</v>
+      </c>
+      <c r="C38" s="19" t="s">
+        <v>86</v>
+      </c>
+      <c r="D38" s="9"/>
+      <c r="E38" s="9"/>
+      <c r="F38" s="9"/>
+      <c r="G38" s="10" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A39" s="19" t="s">
+        <v>67</v>
+      </c>
+      <c r="B39" s="19">
+        <v>614</v>
+      </c>
+      <c r="C39" s="19" t="s">
+        <v>87</v>
+      </c>
+      <c r="D39" s="9"/>
+      <c r="E39" s="9"/>
+      <c r="F39" s="9"/>
+      <c r="G39" s="10" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A40" s="19" t="s">
+        <v>68</v>
+      </c>
+      <c r="B40" s="19">
+        <v>615</v>
+      </c>
+      <c r="C40" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="D40" s="9"/>
+      <c r="E40" s="9"/>
+      <c r="F40" s="9"/>
+      <c r="G40" s="10" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A41" s="19" t="s">
+        <v>69</v>
+      </c>
+      <c r="B41" s="19">
+        <v>615</v>
+      </c>
+      <c r="C41" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="D41" s="9"/>
+      <c r="E41" s="9"/>
+      <c r="F41" s="9"/>
+      <c r="G41" s="10" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A42" s="19" t="s">
+        <v>70</v>
+      </c>
+      <c r="B42" s="19">
+        <v>615</v>
+      </c>
+      <c r="C42" s="19" t="s">
+        <v>86</v>
+      </c>
+      <c r="D42" s="9"/>
+      <c r="E42" s="9"/>
+      <c r="F42" s="9"/>
+      <c r="G42" s="10" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A43" s="19" t="s">
+        <v>71</v>
+      </c>
+      <c r="B43" s="19">
+        <v>615</v>
+      </c>
+      <c r="C43" s="19" t="s">
+        <v>87</v>
+      </c>
+      <c r="D43" s="9"/>
+      <c r="E43" s="9"/>
+      <c r="F43" s="9"/>
+      <c r="G43" s="10" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A44" s="19" t="s">
+        <v>72</v>
+      </c>
+      <c r="B44" s="19">
+        <v>616</v>
+      </c>
+      <c r="C44" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="D44" s="9"/>
+      <c r="E44" s="9"/>
+      <c r="F44" s="9"/>
+      <c r="G44" s="10" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A45" s="19" t="s">
+        <v>73</v>
+      </c>
+      <c r="B45" s="19">
+        <v>616</v>
+      </c>
+      <c r="C45" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="D45" s="9"/>
+      <c r="E45" s="9"/>
+      <c r="F45" s="9"/>
+      <c r="G45" s="10" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A46" s="19" t="s">
+        <v>74</v>
+      </c>
+      <c r="B46" s="19">
+        <v>616</v>
+      </c>
+      <c r="C46" s="19" t="s">
+        <v>86</v>
+      </c>
+      <c r="D46" s="9"/>
+      <c r="E46" s="9"/>
+      <c r="F46" s="9"/>
+      <c r="G46" s="10" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A47" s="19" t="s">
+        <v>75</v>
+      </c>
+      <c r="B47" s="19">
+        <v>616</v>
+      </c>
+      <c r="C47" s="19" t="s">
+        <v>87</v>
+      </c>
+      <c r="D47" s="9"/>
+      <c r="E47" s="9"/>
+      <c r="F47" s="9"/>
+      <c r="G47" s="10" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A48" s="19" t="s">
+        <v>76</v>
+      </c>
+      <c r="B48" s="19">
+        <v>617</v>
+      </c>
+      <c r="C48" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="D48" s="9"/>
+      <c r="E48" s="9"/>
+      <c r="F48" s="9"/>
+      <c r="G48" s="10" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A49" s="19" t="s">
+        <v>77</v>
+      </c>
+      <c r="B49" s="19">
+        <v>617</v>
+      </c>
+      <c r="C49" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="D49" s="9"/>
+      <c r="E49" s="9"/>
+      <c r="F49" s="9"/>
+      <c r="G49" s="10" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A50" s="19" t="s">
+        <v>78</v>
+      </c>
+      <c r="B50" s="19">
+        <v>617</v>
+      </c>
+      <c r="C50" s="19" t="s">
+        <v>86</v>
+      </c>
+      <c r="D50" s="9"/>
+      <c r="E50" s="9"/>
+      <c r="F50" s="9"/>
+      <c r="G50" s="10" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A51" s="19" t="s">
+        <v>79</v>
+      </c>
+      <c r="B51" s="19">
+        <v>617</v>
+      </c>
+      <c r="C51" s="19" t="s">
+        <v>87</v>
+      </c>
+      <c r="D51" s="9"/>
+      <c r="E51" s="9"/>
+      <c r="F51" s="9"/>
+      <c r="G51" s="10" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A52" s="19" t="s">
+        <v>80</v>
+      </c>
+      <c r="B52" s="19">
+        <v>620</v>
+      </c>
+      <c r="C52" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="D52" s="9"/>
+      <c r="E52" s="9"/>
+      <c r="F52" s="9"/>
+      <c r="G52" s="10" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A53" s="19" t="s">
+        <v>81</v>
+      </c>
+      <c r="B53" s="19">
+        <v>620</v>
+      </c>
+      <c r="C53" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="D53" s="9"/>
+      <c r="E53" s="9"/>
+      <c r="F53" s="9"/>
+      <c r="G53" s="10" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A54" s="19" t="s">
+        <v>82</v>
+      </c>
+      <c r="B54" s="19">
+        <v>620</v>
+      </c>
+      <c r="C54" s="19" t="s">
+        <v>86</v>
+      </c>
+      <c r="D54" s="9"/>
+      <c r="E54" s="9"/>
+      <c r="F54" s="9"/>
+      <c r="G54" s="10" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A55" s="19" t="s">
+        <v>83</v>
+      </c>
+      <c r="B55" s="19">
+        <v>620</v>
+      </c>
+      <c r="C55" s="19" t="s">
+        <v>87</v>
+      </c>
+      <c r="D55" s="9"/>
+      <c r="E55" s="9"/>
+      <c r="F55" s="9"/>
+      <c r="G55" s="10" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A56" s="19" t="s">
+        <v>84</v>
+      </c>
+      <c r="B56" s="19">
+        <v>620</v>
+      </c>
+      <c r="C56" s="19" t="s">
+        <v>88</v>
+      </c>
+      <c r="D56" s="9"/>
+      <c r="E56" s="9"/>
+      <c r="F56" s="9"/>
+      <c r="G56" s="10" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A57" s="19" t="s">
+        <v>85</v>
+      </c>
+      <c r="B57" s="19">
+        <v>620</v>
+      </c>
+      <c r="C57" s="19" t="s">
+        <v>89</v>
+      </c>
+      <c r="D57" s="9"/>
+      <c r="E57" s="9"/>
+      <c r="F57" s="9"/>
+      <c r="G57" s="10" t="s">
+        <v>90</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="7">
+    <mergeCell ref="A1:G1"/>
     <mergeCell ref="J4:K4"/>
     <mergeCell ref="L4:M4"/>
     <mergeCell ref="D3:E3"/>
     <mergeCell ref="D2:E2"/>
     <mergeCell ref="B3:C3"/>
     <mergeCell ref="B2:C2"/>
-    <mergeCell ref="A1:G1"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B3" r:id="rId1" xr:uid="{B14FA537-6AA0-F34E-A6CC-272F9F011B52}"/>

</xml_diff>